<commit_message>
modified code and results
</commit_message>
<xml_diff>
--- a/Titanic_DL/Titanic_DL_result.xlsx
+++ b/Titanic_DL/Titanic_DL_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds030\Desktop\github\Titanic\Titanic_DL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC0517C-110D-48D1-AEED-3922605357C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDF294A-DE8C-4F7B-A4AF-D4D8B2500E00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DD7DFFA-55C1-4FF2-81BD-621110AE4683}"/>
   </bookViews>
@@ -441,9 +441,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -484,6 +481,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -803,20 +803,20 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21" style="14" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="20.25" style="15" customWidth="1"/>
-    <col min="6" max="6" width="16.58203125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11" style="15" customWidth="1"/>
-    <col min="9" max="9" width="59.6640625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="21" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="20.25" style="14" customWidth="1"/>
+    <col min="6" max="6" width="16.58203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="11" style="14" customWidth="1"/>
+    <col min="9" max="9" width="59.6640625" style="14" customWidth="1"/>
     <col min="10" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -848,733 +848,719 @@
       <c r="I1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="17" t="s">
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <v>100</v>
       </c>
-      <c r="D2" s="17">
-        <v>10</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="17">
+      <c r="D2" s="16">
+        <v>10</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="16">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="16">
         <v>1000</v>
       </c>
-      <c r="D3" s="17">
-        <v>10</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="17">
+      <c r="D3" s="16">
+        <v>10</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="16">
         <v>0.72726999999999997</v>
       </c>
-      <c r="I3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="20" t="s">
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>500</v>
       </c>
-      <c r="D4" s="20">
-        <v>10</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="20">
+      <c r="D4" s="19">
+        <v>10</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="19">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>280</v>
       </c>
-      <c r="D5" s="20">
-        <v>10</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="20">
+      <c r="D5" s="19">
+        <v>10</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="19">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="20" t="s">
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>800</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="20">
+      <c r="E6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="20" t="s">
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>600</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <v>1</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="20">
+      <c r="E7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="20" t="s">
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>300</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <v>1</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="20">
+      <c r="E8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="19">
         <v>0.75119000000000002</v>
       </c>
-      <c r="I8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="20" t="s">
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>200</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="19">
         <v>1</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="20">
+      <c r="E9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="19">
         <v>0.75597999999999999</v>
       </c>
-      <c r="I9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="20" t="s">
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <v>100</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="19">
         <v>1</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="20">
+      <c r="E10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="19">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="17" t="s">
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>1000</v>
       </c>
-      <c r="D11" s="17">
-        <v>10</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="17">
+      <c r="D11" s="16">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="16">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="17" t="s">
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>500</v>
       </c>
-      <c r="D12" s="17">
-        <v>10</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="17">
+      <c r="D12" s="16">
+        <v>10</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="16">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="17" t="s">
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>200</v>
       </c>
-      <c r="D13" s="17">
-        <v>10</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="17">
+      <c r="D13" s="16">
+        <v>10</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="16">
         <v>0.76075999999999999</v>
       </c>
-      <c r="I13" s="17"/>
-    </row>
-    <row r="14" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="17" t="s">
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>100</v>
       </c>
-      <c r="D14" s="17">
-        <v>10</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="17">
+      <c r="D14" s="16">
+        <v>10</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="17" t="s">
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>90</v>
       </c>
-      <c r="D15" s="17">
-        <v>10</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="17">
+      <c r="D15" s="16">
+        <v>10</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="17" t="s">
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>70</v>
       </c>
-      <c r="D16" s="17">
-        <v>10</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="17">
+      <c r="D16" s="16">
+        <v>10</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I16" s="17"/>
-    </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="17" t="s">
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="16">
         <v>50</v>
       </c>
-      <c r="D17" s="17">
-        <v>10</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="17">
+      <c r="D17" s="16">
+        <v>10</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="16">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <v>500</v>
       </c>
-      <c r="D18" s="20">
-        <v>10</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="20">
-        <v>0.73684000000000005</v>
-      </c>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="20" t="s">
+      <c r="D18" s="19">
+        <v>10</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="19">
         <v>200</v>
       </c>
-      <c r="D19" s="20">
-        <v>10</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="20">
+      <c r="D19" s="19">
+        <v>10</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="19">
+        <v>100</v>
+      </c>
+      <c r="D20" s="19">
+        <v>10</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="16">
+        <v>500</v>
+      </c>
+      <c r="D21" s="16">
+        <v>10</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="16">
+        <v>300</v>
+      </c>
+      <c r="D22" s="16">
+        <v>10</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="16">
+        <v>200</v>
+      </c>
+      <c r="D23" s="16">
+        <v>10</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="16">
+        <v>100</v>
+      </c>
+      <c r="D24" s="16">
+        <v>10</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="19">
+        <v>500</v>
+      </c>
+      <c r="D25" s="19">
+        <v>10</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="19">
+        <v>0.72726999999999997</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="19">
+        <v>200</v>
+      </c>
+      <c r="D26" s="19">
+        <v>10</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I19" s="20"/>
-    </row>
-    <row r="20" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="20">
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="16">
+        <v>500</v>
+      </c>
+      <c r="D27" s="16">
+        <v>10</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0.72248000000000001</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="16">
         <v>100</v>
       </c>
-      <c r="D20" s="20">
-        <v>10</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="20">
-        <v>0.70813000000000004</v>
-      </c>
-      <c r="I20" s="20"/>
-    </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="17">
-        <v>500</v>
-      </c>
-      <c r="D21" s="17">
-        <v>10</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="17">
-        <v>0.73204999999999998</v>
-      </c>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="17">
-        <v>300</v>
-      </c>
-      <c r="D22" s="17">
-        <v>10</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="17">
-        <v>0.75119000000000002</v>
-      </c>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="17">
-        <v>200</v>
-      </c>
-      <c r="D23" s="17">
-        <v>10</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="17">
-        <v>0.75597999999999999</v>
-      </c>
-      <c r="I23" s="17"/>
-    </row>
-    <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="17">
-        <v>100</v>
-      </c>
-      <c r="D24" s="17">
-        <v>10</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="17">
-        <v>0.74161999999999995</v>
-      </c>
-      <c r="I24" s="17"/>
-    </row>
-    <row r="25" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="20">
-        <v>500</v>
-      </c>
-      <c r="D25" s="20">
-        <v>10</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="20">
-        <v>0.72726999999999997</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="20">
-        <v>200</v>
-      </c>
-      <c r="D26" s="20">
-        <v>10</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="20">
-        <v>0.74161999999999995</v>
-      </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="17">
-        <v>500</v>
-      </c>
-      <c r="D27" s="17">
-        <v>10</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="17">
-        <v>0.72248000000000001</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="17">
-        <v>100</v>
-      </c>
-      <c r="D28" s="17">
-        <v>10</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="17">
+      <c r="D28" s="16">
+        <v>10</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="16">
         <v>0.73204999999999998</v>
       </c>
     </row>
@@ -1601,10 +1587,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="7"/>
+      <c r="A1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="21"/>
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1701,13 +1687,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1737,72 +1723,72 @@
       <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new comment about the results
</commit_message>
<xml_diff>
--- a/Titanic_DL/Titanic_DL_result.xlsx
+++ b/Titanic_DL/Titanic_DL_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds030\Desktop\github\Titanic\Titanic_DL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D736F0-97C4-4A41-B596-AE32B2687153}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545F9A8F-C558-429D-902C-728AFF128D02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DD7DFFA-55C1-4FF2-81BD-621110AE4683}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="63">
   <si>
     <t>model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -266,6 +266,107 @@
   </si>
   <si>
     <t>model1보다 더 간단한 모델</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model1과는 최악의 조합</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">100번 학습했을 때 가장 성능이 좋으므로
+학습을 조금만 시켰을 때 더 좋은 성능을 내는지 확인
+-&gt; 100~200사이도 확인해봐야겠다.
+--&gt; 160 to 165: 5 epoch 동안 큰 변화가 있어보인다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>좀 더 단순한 모델</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>을 만들어봐야겠다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>batch사이즈를 줄이면 더 섬세한 특징을 잡아서
+성능이 더 높아지지 않을까해서 batch size=1로 학습시켜봄
+-&gt; 1이나 10이나 둘 다 작은 사이즈라 별반 차이가 없는 듯하다.
+일단</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> batch size를 10으로 통일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>하자</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">점수가 너무 낮으므로
+혹시 학습을 조금만 시켰을 때 더 좋은 성능을 내는 것인지 확인
+-&gt; feature6_3  ['Pclass', 'Name','Age','Family','Fare', 'Cabin_s']
+은  일단 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>model1과는 좋은 성능을 내지못하는 것</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>을 확인함</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -273,7 +374,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +387,23 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -464,7 +582,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -547,6 +665,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -863,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0566AD2C-C438-4E84-84A1-D7FB43D10CCE}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -992,7 +1131,9 @@
       <c r="H4" s="19">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I4" s="19"/>
+      <c r="I4" s="33" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="18" t="s">
@@ -1019,7 +1160,7 @@
       <c r="H5" s="19">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I5" s="19"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
@@ -1046,7 +1187,7 @@
       <c r="H6" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I6" s="19"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
@@ -1073,7 +1214,7 @@
       <c r="H7" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
@@ -1100,7 +1241,7 @@
       <c r="H8" s="19">
         <v>0.75119000000000002</v>
       </c>
-      <c r="I8" s="19"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
@@ -1127,7 +1268,7 @@
       <c r="H9" s="19">
         <v>0.75597999999999999</v>
       </c>
-      <c r="I9" s="19"/>
+      <c r="I9" s="32"/>
     </row>
     <row r="10" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
@@ -1154,7 +1295,7 @@
       <c r="H10" s="19">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I10" s="19"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
@@ -1181,7 +1322,9 @@
       <c r="H11" s="16">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="31" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
@@ -1208,7 +1351,7 @@
       <c r="H12" s="16">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I12" s="16"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
@@ -1235,7 +1378,7 @@
       <c r="H13" s="16">
         <v>0.76075999999999999</v>
       </c>
-      <c r="I13" s="16"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
@@ -1245,7 +1388,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="16">
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="D14" s="16">
         <v>10</v>
@@ -1259,10 +1402,10 @@
       <c r="G14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="16">
-        <v>0.77510999999999997</v>
-      </c>
-      <c r="I14" s="16"/>
+      <c r="H14" s="34">
+        <v>0.74641000000000002</v>
+      </c>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
@@ -1272,7 +1415,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="16">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="D15" s="16">
         <v>10</v>
@@ -1286,10 +1429,10 @@
       <c r="G15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="16">
-        <v>0.77510999999999997</v>
-      </c>
-      <c r="I15" s="16"/>
+      <c r="H15" s="34">
+        <v>0.73204999999999998</v>
+      </c>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
@@ -1299,7 +1442,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="16">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="D16" s="16">
         <v>10</v>
@@ -1313,10 +1456,10 @@
       <c r="G16" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="16">
-        <v>0.77510999999999997</v>
-      </c>
-      <c r="I16" s="16"/>
+      <c r="H16" s="34">
+        <v>0.77032999999999996</v>
+      </c>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
@@ -1326,142 +1469,142 @@
         <v>26</v>
       </c>
       <c r="C17" s="16">
+        <v>100</v>
+      </c>
+      <c r="D17" s="16">
+        <v>10</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="16">
+        <v>0.77510999999999997</v>
+      </c>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="16">
+        <v>90</v>
+      </c>
+      <c r="D18" s="16">
+        <v>10</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="16">
+        <v>0.77510999999999997</v>
+      </c>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="16">
+        <v>70</v>
+      </c>
+      <c r="D19" s="16">
+        <v>10</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="16">
+        <v>0.77510999999999997</v>
+      </c>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="16">
         <v>50</v>
       </c>
-      <c r="D17" s="16">
-        <v>10</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="16">
+      <c r="D20" s="16">
+        <v>10</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="16">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="19">
-        <v>500</v>
-      </c>
-      <c r="D18" s="19">
-        <v>10</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="19">
-        <v>0.74641000000000002</v>
-      </c>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="19">
-        <v>300</v>
-      </c>
-      <c r="D19" s="19">
-        <v>10</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="19">
-        <v>0.76554999999999995</v>
-      </c>
-      <c r="I19" s="19"/>
-    </row>
-    <row r="20" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="19">
-        <v>200</v>
-      </c>
-      <c r="D20" s="19">
-        <v>10</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="19">
-        <v>0.76554999999999995</v>
-      </c>
-      <c r="I20" s="19"/>
-    </row>
-    <row r="21" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="19">
-        <v>100</v>
-      </c>
-      <c r="D21" s="19">
-        <v>10</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="19">
-        <v>0.7177</v>
-      </c>
-      <c r="I21" s="19"/>
+      <c r="I20" s="30"/>
+    </row>
+    <row r="21" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="16">
+        <v>40</v>
+      </c>
+      <c r="D21" s="16">
+        <v>10</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0.71291000000000004</v>
+      </c>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C22" s="16">
-        <v>600</v>
+        <v>20</v>
       </c>
       <c r="D22" s="16">
         <v>10</v>
@@ -1476,100 +1619,100 @@
         <v>22</v>
       </c>
       <c r="H22" s="16">
+        <v>0.69377</v>
+      </c>
+      <c r="I22" s="30"/>
+    </row>
+    <row r="23" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="19">
+        <v>500</v>
+      </c>
+      <c r="D23" s="19">
+        <v>10</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="19">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I22" s="16"/>
-    </row>
-    <row r="23" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="16">
-        <v>500</v>
-      </c>
-      <c r="D23" s="16">
-        <v>10</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0.75597999999999999</v>
-      </c>
-      <c r="I23" s="16"/>
-    </row>
-    <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="16">
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="19">
+        <v>300</v>
+      </c>
+      <c r="D24" s="19">
+        <v>10</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="19">
+        <v>0.76554999999999995</v>
+      </c>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="19">
         <v>200</v>
       </c>
-      <c r="D24" s="16">
-        <v>10</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="16">
-        <v>0.75119000000000002</v>
-      </c>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="16">
-        <v>100</v>
-      </c>
-      <c r="D25" s="16">
-        <v>10</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0.73684000000000005</v>
-      </c>
-      <c r="I25" s="16"/>
+      <c r="D25" s="19">
+        <v>10</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="19">
+        <v>0.76554999999999995</v>
+      </c>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C26" s="19">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D26" s="19">
         <v>10</v>
@@ -1584,43 +1727,43 @@
         <v>22</v>
       </c>
       <c r="H26" s="19">
-        <v>0.72726999999999997</v>
+        <v>0.7177</v>
       </c>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="19">
-        <v>200</v>
-      </c>
-      <c r="D27" s="19">
-        <v>10</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="19">
-        <v>0.74161999999999995</v>
-      </c>
-      <c r="I27" s="19"/>
+    <row r="27" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="16">
+        <v>600</v>
+      </c>
+      <c r="D27" s="16">
+        <v>10</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0.74641000000000002</v>
+      </c>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C28" s="16">
         <v>500</v>
@@ -1638,168 +1781,170 @@
         <v>22</v>
       </c>
       <c r="H28" s="16">
+        <v>0.75597999999999999</v>
+      </c>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="16">
+        <v>200</v>
+      </c>
+      <c r="D29" s="16">
+        <v>10</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0.75119000000000002</v>
+      </c>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="16">
+        <v>100</v>
+      </c>
+      <c r="D30" s="16">
+        <v>10</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="16">
+        <v>0.73684000000000005</v>
+      </c>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="19">
+        <v>500</v>
+      </c>
+      <c r="D31" s="19">
+        <v>10</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="19">
+        <v>0.72726999999999997</v>
+      </c>
+      <c r="I31" s="19"/>
+    </row>
+    <row r="32" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="19">
+        <v>200</v>
+      </c>
+      <c r="D32" s="19">
+        <v>10</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="19">
+        <v>0.74161999999999995</v>
+      </c>
+      <c r="I32" s="19"/>
+    </row>
+    <row r="33" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="16">
+        <v>500</v>
+      </c>
+      <c r="D33" s="16">
+        <v>10</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="16">
         <v>0.72248000000000001</v>
       </c>
-      <c r="I28" s="16"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="16" t="s">
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C34" s="16">
         <v>100</v>
       </c>
-      <c r="D29" s="16">
-        <v>10</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="16">
+      <c r="D34" s="16">
+        <v>10</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="16">
         <v>0.73204999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="22">
-        <v>600</v>
-      </c>
-      <c r="D30" s="22">
-        <v>10</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30" s="22">
-        <v>0.3</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="22">
-        <v>0.66984999999999995</v>
-      </c>
-      <c r="I30" s="22"/>
-    </row>
-    <row r="31" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="22">
-        <v>300</v>
-      </c>
-      <c r="D31" s="22">
-        <v>10</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="22">
-        <v>0.3</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="22">
-        <v>0.71291000000000004</v>
-      </c>
-      <c r="I31" s="22"/>
-    </row>
-    <row r="32" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="22">
-        <v>200</v>
-      </c>
-      <c r="D32" s="22">
-        <v>10</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="22">
-        <v>0.3</v>
-      </c>
-      <c r="G32" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="22">
-        <v>0.72248000000000001</v>
-      </c>
-      <c r="I32" s="22"/>
-    </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="22">
-        <v>100</v>
-      </c>
-      <c r="D33" s="22">
-        <v>10</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="22">
-        <v>0.3</v>
-      </c>
-      <c r="G33" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" s="22">
-        <v>0.71291000000000004</v>
-      </c>
-      <c r="I33" s="22"/>
-    </row>
-    <row r="34" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="22">
-        <v>80</v>
-      </c>
-      <c r="D34" s="22">
-        <v>10</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="22">
-        <v>0.3</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="21" t="s">
@@ -1809,7 +1954,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="22">
-        <v>50</v>
+        <v>600</v>
       </c>
       <c r="D35" s="22">
         <v>10</v>
@@ -1824,9 +1969,11 @@
         <v>22</v>
       </c>
       <c r="H35" s="22">
-        <v>0.70813000000000004</v>
-      </c>
-      <c r="I35" s="22"/>
+        <v>0.66984999999999995</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="21" t="s">
@@ -1836,7 +1983,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="22">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="D36" s="22">
         <v>10</v>
@@ -1851,9 +1998,9 @@
         <v>22</v>
       </c>
       <c r="H36" s="22">
-        <v>0.69377</v>
-      </c>
-      <c r="I36" s="22"/>
+        <v>0.71291000000000004</v>
+      </c>
+      <c r="I36" s="28"/>
     </row>
     <row r="37" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
@@ -1863,161 +2010,161 @@
         <v>34</v>
       </c>
       <c r="C37" s="22">
+        <v>200</v>
+      </c>
+      <c r="D37" s="22">
+        <v>10</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="22">
+        <v>0.72248000000000001</v>
+      </c>
+      <c r="I37" s="28"/>
+    </row>
+    <row r="38" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="22">
+        <v>100</v>
+      </c>
+      <c r="D38" s="22">
+        <v>10</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="22">
+        <v>0.71291000000000004</v>
+      </c>
+      <c r="I38" s="28"/>
+    </row>
+    <row r="39" spans="1:9" s="23" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="29">
+        <v>80</v>
+      </c>
+      <c r="D39" s="22">
+        <v>10</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="22">
+        <v>0.67942000000000002</v>
+      </c>
+      <c r="I39" s="28"/>
+    </row>
+    <row r="40" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="29">
+        <v>50</v>
+      </c>
+      <c r="D40" s="22">
+        <v>10</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="22">
+        <v>0.70813000000000004</v>
+      </c>
+      <c r="I40" s="28"/>
+    </row>
+    <row r="41" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="29">
+        <v>20</v>
+      </c>
+      <c r="D41" s="22">
+        <v>10</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="22">
+        <v>0.69377</v>
+      </c>
+      <c r="I41" s="28"/>
+    </row>
+    <row r="42" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="29">
         <v>5</v>
       </c>
-      <c r="D37" s="22">
-        <v>10</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="22">
-        <v>0.3</v>
-      </c>
-      <c r="G37" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="22">
+      <c r="D42" s="22">
+        <v>10</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="22">
         <v>0.69855999999999996</v>
       </c>
-      <c r="I37" s="22"/>
-    </row>
-    <row r="38" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="16">
-        <v>600</v>
-      </c>
-      <c r="D38" s="16">
-        <v>10</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="16">
-        <v>0.75119000000000002</v>
-      </c>
-      <c r="I38" s="16"/>
-    </row>
-    <row r="39" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="16">
-        <v>500</v>
-      </c>
-      <c r="D39" s="16">
-        <v>10</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="16">
-        <v>0.76075999999999999</v>
-      </c>
-      <c r="I39" s="16"/>
-    </row>
-    <row r="40" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="16">
-        <v>400</v>
-      </c>
-      <c r="D40" s="16">
-        <v>10</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H40" s="16">
-        <v>0.77032999999999996</v>
-      </c>
-      <c r="I40" s="16"/>
-    </row>
-    <row r="41" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="16">
-        <v>300</v>
-      </c>
-      <c r="D41" s="16">
-        <v>10</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H41" s="16">
-        <v>0.75119000000000002</v>
-      </c>
-      <c r="I41" s="16"/>
-    </row>
-    <row r="42" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="16">
-        <v>200</v>
-      </c>
-      <c r="D42" s="16">
-        <v>10</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="16">
-        <v>0.73684000000000005</v>
-      </c>
-      <c r="I42" s="16"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I42" s="28"/>
+    </row>
+    <row r="43" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
         <v>7</v>
       </c>
@@ -2025,25 +2172,165 @@
         <v>35</v>
       </c>
       <c r="C43" s="16">
+        <v>600</v>
+      </c>
+      <c r="D43" s="16">
+        <v>10</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="16">
+        <v>0.75119000000000002</v>
+      </c>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="16">
+        <v>500</v>
+      </c>
+      <c r="D44" s="16">
+        <v>10</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="16">
+        <v>0.76075999999999999</v>
+      </c>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="16">
+        <v>400</v>
+      </c>
+      <c r="D45" s="16">
+        <v>10</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="16">
+        <v>0.77032999999999996</v>
+      </c>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="16">
+        <v>300</v>
+      </c>
+      <c r="D46" s="16">
+        <v>10</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="16">
+        <v>0.75119000000000002</v>
+      </c>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="16">
+        <v>200</v>
+      </c>
+      <c r="D47" s="16">
+        <v>10</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="16">
+        <v>0.73684000000000005</v>
+      </c>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A48" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="16">
         <v>100</v>
       </c>
-      <c r="D43" s="16">
-        <v>10</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H43" s="16">
+      <c r="D48" s="16">
+        <v>10</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="16">
         <v>0.71291000000000004</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I35:I42"/>
+    <mergeCell ref="I11:I22"/>
+    <mergeCell ref="I4:I10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -2196,14 +2483,14 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="20.25" customWidth="1"/>
     <col min="2" max="2" width="80.4140625" customWidth="1"/>
-    <col min="3" max="3" width="18.58203125" customWidth="1"/>
+    <col min="3" max="3" width="42.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -2302,6 +2589,9 @@
       </c>
       <c r="B11" s="8" t="s">
         <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
upload new file and modified ReadMe
</commit_message>
<xml_diff>
--- a/Titanic_DL/Titanic_DL_result.xlsx
+++ b/Titanic_DL/Titanic_DL_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds030\Desktop\github\Titanic\Titanic_DL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D229F5-5CFB-4497-981E-6763442A09ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CE0263-C733-4231-B0E7-E6C141F29B59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DD7DFFA-55C1-4FF2-81BD-621110AE4683}"/>
+    <workbookView xWindow="-6880" yWindow="3030" windowWidth="14400" windowHeight="7360" xr2:uid="{7DD7DFFA-55C1-4FF2-81BD-621110AE4683}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
@@ -744,9 +744,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -759,6 +774,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,27 +790,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0566AD2C-C438-4E84-84A1-D7FB43D10CCE}">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1235,7 +1235,7 @@
       <c r="H4" s="19">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="38" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
       <c r="H5" s="19">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
@@ -1291,7 +1291,7 @@
       <c r="H6" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I6" s="34"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
@@ -1318,7 +1318,7 @@
       <c r="H7" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I7" s="34"/>
+      <c r="I7" s="39"/>
     </row>
     <row r="8" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
@@ -1345,7 +1345,7 @@
       <c r="H8" s="19">
         <v>0.75119000000000002</v>
       </c>
-      <c r="I8" s="34"/>
+      <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
@@ -1372,7 +1372,7 @@
       <c r="H9" s="19">
         <v>0.75597999999999999</v>
       </c>
-      <c r="I9" s="34"/>
+      <c r="I9" s="39"/>
     </row>
     <row r="10" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
@@ -1399,7 +1399,7 @@
       <c r="H10" s="19">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="39"/>
     </row>
     <row r="11" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
@@ -1426,7 +1426,7 @@
       <c r="H11" s="16">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="36" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       <c r="H12" s="16">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I12" s="32"/>
+      <c r="I12" s="37"/>
     </row>
     <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
@@ -1482,7 +1482,7 @@
       <c r="H13" s="16">
         <v>0.76075999999999999</v>
       </c>
-      <c r="I13" s="32"/>
+      <c r="I13" s="37"/>
     </row>
     <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
@@ -1509,7 +1509,7 @@
       <c r="H14" s="25">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
@@ -1536,7 +1536,7 @@
       <c r="H15" s="25">
         <v>0.73204999999999998</v>
       </c>
-      <c r="I15" s="32"/>
+      <c r="I15" s="37"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
@@ -1563,7 +1563,7 @@
       <c r="H16" s="25">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I16" s="32"/>
+      <c r="I16" s="37"/>
     </row>
     <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
@@ -1590,7 +1590,7 @@
       <c r="H17" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I17" s="32"/>
+      <c r="I17" s="37"/>
     </row>
     <row r="18" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
@@ -1617,7 +1617,7 @@
       <c r="H18" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I18" s="32"/>
+      <c r="I18" s="37"/>
     </row>
     <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
@@ -1644,7 +1644,7 @@
       <c r="H19" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I19" s="32"/>
+      <c r="I19" s="37"/>
     </row>
     <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
@@ -1671,7 +1671,7 @@
       <c r="H20" s="16">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I20" s="32"/>
+      <c r="I20" s="37"/>
     </row>
     <row r="21" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
@@ -1698,7 +1698,7 @@
       <c r="H21" s="16">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I21" s="32"/>
+      <c r="I21" s="37"/>
     </row>
     <row r="22" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
@@ -1725,7 +1725,7 @@
       <c r="H22" s="16">
         <v>0.69377</v>
       </c>
-      <c r="I22" s="32"/>
+      <c r="I22" s="37"/>
     </row>
     <row r="23" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
@@ -2075,7 +2075,7 @@
       <c r="H35" s="22">
         <v>0.66984999999999995</v>
       </c>
-      <c r="I35" s="30" t="s">
+      <c r="I35" s="34" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2104,7 +2104,7 @@
       <c r="H36" s="22">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I36" s="30"/>
+      <c r="I36" s="34"/>
     </row>
     <row r="37" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
@@ -2131,7 +2131,7 @@
       <c r="H37" s="22">
         <v>0.72248000000000001</v>
       </c>
-      <c r="I37" s="30"/>
+      <c r="I37" s="34"/>
     </row>
     <row r="38" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="21" t="s">
@@ -2158,7 +2158,7 @@
       <c r="H38" s="22">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I38" s="30"/>
+      <c r="I38" s="34"/>
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
@@ -2185,7 +2185,7 @@
       <c r="H39" s="22">
         <v>0.67942000000000002</v>
       </c>
-      <c r="I39" s="30"/>
+      <c r="I39" s="34"/>
     </row>
     <row r="40" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="21" t="s">
@@ -2212,7 +2212,7 @@
       <c r="H40" s="22">
         <v>0.70813000000000004</v>
       </c>
-      <c r="I40" s="30"/>
+      <c r="I40" s="34"/>
     </row>
     <row r="41" spans="1:9" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="21" t="s">
@@ -2239,7 +2239,7 @@
       <c r="H41" s="22">
         <v>0.69377</v>
       </c>
-      <c r="I41" s="30"/>
+      <c r="I41" s="34"/>
     </row>
     <row r="42" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="21" t="s">
@@ -2266,7 +2266,7 @@
       <c r="H42" s="22">
         <v>0.69855999999999996</v>
       </c>
-      <c r="I42" s="30"/>
+      <c r="I42" s="34"/>
     </row>
     <row r="43" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
@@ -2643,7 +2643,7 @@
       <c r="H56" s="26">
         <v>0.69377</v>
       </c>
-      <c r="I56" s="32"/>
+      <c r="I56" s="37"/>
     </row>
     <row r="57" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="15" t="s">
@@ -2670,7 +2670,7 @@
       <c r="H57" s="28">
         <v>0.66027999999999998</v>
       </c>
-      <c r="I57" s="32"/>
+      <c r="I57" s="37"/>
     </row>
     <row r="58" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="15" t="s">
@@ -2697,7 +2697,7 @@
       <c r="H58" s="28">
         <v>0.67464000000000002</v>
       </c>
-      <c r="I58" s="32"/>
+      <c r="I58" s="37"/>
     </row>
     <row r="59" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="15" t="s">
@@ -2724,7 +2724,7 @@
       <c r="H59" s="28">
         <v>0.7177</v>
       </c>
-      <c r="I59" s="32"/>
+      <c r="I59" s="37"/>
     </row>
     <row r="60" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="15" t="s">
@@ -2751,7 +2751,7 @@
       <c r="H60" s="28">
         <v>0.72726999999999997</v>
       </c>
-      <c r="I60" s="32"/>
+      <c r="I60" s="37"/>
     </row>
     <row r="61" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="15" t="s">
@@ -2778,7 +2778,7 @@
       <c r="H61" s="28">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I61" s="32"/>
+      <c r="I61" s="37"/>
     </row>
     <row r="62" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="15" t="s">
@@ -2805,7 +2805,7 @@
       <c r="H62" s="26">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I62" s="32"/>
+      <c r="I62" s="37"/>
     </row>
     <row r="63" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="15" t="s">
@@ -2832,34 +2832,34 @@
       <c r="H63" s="28">
         <v>0.72726999999999997</v>
       </c>
-      <c r="I63" s="32"/>
-    </row>
-    <row r="64" spans="1:9" s="41" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" s="40" t="s">
+      <c r="I63" s="37"/>
+    </row>
+    <row r="64" spans="1:9" s="32" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A64" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="40">
+      <c r="C64" s="31">
         <v>100</v>
       </c>
-      <c r="D64" s="40">
-        <v>10</v>
-      </c>
-      <c r="E64" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" s="40">
-        <v>0.3</v>
-      </c>
-      <c r="G64" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="H64" s="40">
+      <c r="D64" s="31">
+        <v>10</v>
+      </c>
+      <c r="E64" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="31">
+        <v>0.3</v>
+      </c>
+      <c r="G64" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="31">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I64" s="42"/>
+      <c r="I64" s="40"/>
     </row>
     <row r="65" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="21" t="s">
@@ -2886,7 +2886,7 @@
       <c r="H65" s="22">
         <v>0.76075999999999999</v>
       </c>
-      <c r="I65" s="44" t="s">
+      <c r="I65" s="41" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2912,10 +2912,10 @@
       <c r="G66" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H66" s="45">
+      <c r="H66" s="33">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I66" s="43"/>
+      <c r="I66" s="35"/>
     </row>
     <row r="67" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="21" t="s">
@@ -2939,10 +2939,10 @@
       <c r="G67" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H67" s="45">
+      <c r="H67" s="33">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I67" s="43"/>
+      <c r="I67" s="35"/>
     </row>
     <row r="68" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="21" t="s">
@@ -2966,10 +2966,10 @@
       <c r="G68" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H68" s="45">
+      <c r="H68" s="33">
         <v>0.75597999999999999</v>
       </c>
-      <c r="I68" s="43"/>
+      <c r="I68" s="35"/>
     </row>
     <row r="69" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="21" t="s">
@@ -2996,7 +2996,7 @@
       <c r="H69" s="22">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I69" s="43"/>
+      <c r="I69" s="35"/>
     </row>
     <row r="70" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="21" t="s">
@@ -3023,7 +3023,7 @@
       <c r="H70" s="24">
         <v>0.76554999999999995</v>
       </c>
-      <c r="I70" s="30" t="s">
+      <c r="I70" s="34" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3052,7 +3052,7 @@
       <c r="H71" s="24">
         <v>0.79425000000000001</v>
       </c>
-      <c r="I71" s="43"/>
+      <c r="I71" s="35"/>
     </row>
     <row r="72" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="21" t="s">
@@ -3079,7 +3079,7 @@
       <c r="H72" s="24">
         <v>0.77990000000000004</v>
       </c>
-      <c r="I72" s="43"/>
+      <c r="I72" s="35"/>
     </row>
     <row r="73" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="21" t="s">
@@ -3106,7 +3106,7 @@
       <c r="H73" s="24">
         <v>0.78468000000000004</v>
       </c>
-      <c r="I73" s="43"/>
+      <c r="I73" s="35"/>
     </row>
     <row r="74" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="21" t="s">
@@ -3133,7 +3133,7 @@
       <c r="H74" s="24">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I74" s="43"/>
+      <c r="I74" s="35"/>
     </row>
     <row r="75" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="21" t="s">
@@ -3160,7 +3160,7 @@
       <c r="H75" s="24">
         <v>0.78947000000000001</v>
       </c>
-      <c r="I75" s="43"/>
+      <c r="I75" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3181,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961E6CD2-75ED-43C0-A85B-2AC98E43BCA0}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3194,15 +3194,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="35"/>
+      <c r="A1" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="42"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="37"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
@@ -3282,10 +3282,10 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -3322,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435B7095-D6E7-48AC-96FF-B01A9E4C98B1}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
add some DL results
</commit_message>
<xml_diff>
--- a/Titanic_DL/Titanic_DL_result.xlsx
+++ b/Titanic_DL/Titanic_DL_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds030\Desktop\github\Titanic\Titanic_DL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CE0263-C733-4231-B0E7-E6C141F29B59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5635DB59-FCC6-4E07-BEFF-2619E7FB06DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6880" yWindow="3030" windowWidth="14400" windowHeight="7360" xr2:uid="{7DD7DFFA-55C1-4FF2-81BD-621110AE4683}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DD7DFFA-55C1-4FF2-81BD-621110AE4683}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="70">
   <si>
     <t>model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -394,12 +394,20 @@
 102번 학습시켰을 때 가장 성능이 좋다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>model2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature5_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,6 +435,15 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -653,7 +670,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -756,6 +773,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,6 +810,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1106,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0566AD2C-C438-4E84-84A1-D7FB43D10CCE}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1235,7 +1264,7 @@
       <c r="H4" s="19">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="39" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1264,7 +1293,7 @@
       <c r="H5" s="19">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
@@ -1291,7 +1320,7 @@
       <c r="H6" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
@@ -1318,7 +1347,7 @@
       <c r="H7" s="19">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I7" s="39"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
@@ -1345,7 +1374,7 @@
       <c r="H8" s="19">
         <v>0.75119000000000002</v>
       </c>
-      <c r="I8" s="39"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
@@ -1372,7 +1401,7 @@
       <c r="H9" s="19">
         <v>0.75597999999999999</v>
       </c>
-      <c r="I9" s="39"/>
+      <c r="I9" s="40"/>
     </row>
     <row r="10" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
@@ -1399,7 +1428,7 @@
       <c r="H10" s="19">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I10" s="39"/>
+      <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
@@ -1426,7 +1455,7 @@
       <c r="H11" s="16">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="37" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1455,7 +1484,7 @@
       <c r="H12" s="16">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I12" s="37"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
@@ -1482,7 +1511,7 @@
       <c r="H13" s="16">
         <v>0.76075999999999999</v>
       </c>
-      <c r="I13" s="37"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
@@ -1509,7 +1538,7 @@
       <c r="H14" s="25">
         <v>0.74641000000000002</v>
       </c>
-      <c r="I14" s="37"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
@@ -1536,7 +1565,7 @@
       <c r="H15" s="25">
         <v>0.73204999999999998</v>
       </c>
-      <c r="I15" s="37"/>
+      <c r="I15" s="38"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
@@ -1563,7 +1592,7 @@
       <c r="H16" s="25">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I16" s="37"/>
+      <c r="I16" s="38"/>
     </row>
     <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
@@ -1590,7 +1619,7 @@
       <c r="H17" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I17" s="37"/>
+      <c r="I17" s="38"/>
     </row>
     <row r="18" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
@@ -1617,7 +1646,7 @@
       <c r="H18" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I18" s="37"/>
+      <c r="I18" s="38"/>
     </row>
     <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
@@ -1644,7 +1673,7 @@
       <c r="H19" s="16">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I19" s="37"/>
+      <c r="I19" s="38"/>
     </row>
     <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
@@ -1671,7 +1700,7 @@
       <c r="H20" s="16">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I20" s="37"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
@@ -1698,7 +1727,7 @@
       <c r="H21" s="16">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I21" s="37"/>
+      <c r="I21" s="38"/>
     </row>
     <row r="22" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
@@ -1725,7 +1754,7 @@
       <c r="H22" s="16">
         <v>0.69377</v>
       </c>
-      <c r="I22" s="37"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
@@ -2075,7 +2104,7 @@
       <c r="H35" s="22">
         <v>0.66984999999999995</v>
       </c>
-      <c r="I35" s="34" t="s">
+      <c r="I35" s="35" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2104,7 +2133,7 @@
       <c r="H36" s="22">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I36" s="34"/>
+      <c r="I36" s="35"/>
     </row>
     <row r="37" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
@@ -2131,7 +2160,7 @@
       <c r="H37" s="22">
         <v>0.72248000000000001</v>
       </c>
-      <c r="I37" s="34"/>
+      <c r="I37" s="35"/>
     </row>
     <row r="38" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="21" t="s">
@@ -2158,7 +2187,7 @@
       <c r="H38" s="22">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I38" s="34"/>
+      <c r="I38" s="35"/>
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
@@ -2185,7 +2214,7 @@
       <c r="H39" s="22">
         <v>0.67942000000000002</v>
       </c>
-      <c r="I39" s="34"/>
+      <c r="I39" s="35"/>
     </row>
     <row r="40" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="21" t="s">
@@ -2212,7 +2241,7 @@
       <c r="H40" s="22">
         <v>0.70813000000000004</v>
       </c>
-      <c r="I40" s="34"/>
+      <c r="I40" s="35"/>
     </row>
     <row r="41" spans="1:9" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="21" t="s">
@@ -2239,7 +2268,7 @@
       <c r="H41" s="22">
         <v>0.69377</v>
       </c>
-      <c r="I41" s="34"/>
+      <c r="I41" s="35"/>
     </row>
     <row r="42" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="21" t="s">
@@ -2266,7 +2295,7 @@
       <c r="H42" s="22">
         <v>0.69855999999999996</v>
       </c>
-      <c r="I42" s="34"/>
+      <c r="I42" s="35"/>
     </row>
     <row r="43" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
@@ -2643,7 +2672,7 @@
       <c r="H56" s="26">
         <v>0.69377</v>
       </c>
-      <c r="I56" s="37"/>
+      <c r="I56" s="38"/>
     </row>
     <row r="57" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="15" t="s">
@@ -2670,7 +2699,7 @@
       <c r="H57" s="28">
         <v>0.66027999999999998</v>
       </c>
-      <c r="I57" s="37"/>
+      <c r="I57" s="38"/>
     </row>
     <row r="58" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="15" t="s">
@@ -2697,7 +2726,7 @@
       <c r="H58" s="28">
         <v>0.67464000000000002</v>
       </c>
-      <c r="I58" s="37"/>
+      <c r="I58" s="38"/>
     </row>
     <row r="59" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="15" t="s">
@@ -2724,7 +2753,7 @@
       <c r="H59" s="28">
         <v>0.7177</v>
       </c>
-      <c r="I59" s="37"/>
+      <c r="I59" s="38"/>
     </row>
     <row r="60" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="15" t="s">
@@ -2751,7 +2780,7 @@
       <c r="H60" s="28">
         <v>0.72726999999999997</v>
       </c>
-      <c r="I60" s="37"/>
+      <c r="I60" s="38"/>
     </row>
     <row r="61" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="15" t="s">
@@ -2778,7 +2807,7 @@
       <c r="H61" s="28">
         <v>0.74161999999999995</v>
       </c>
-      <c r="I61" s="37"/>
+      <c r="I61" s="38"/>
     </row>
     <row r="62" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="15" t="s">
@@ -2805,7 +2834,7 @@
       <c r="H62" s="26">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I62" s="37"/>
+      <c r="I62" s="38"/>
     </row>
     <row r="63" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="15" t="s">
@@ -2832,7 +2861,7 @@
       <c r="H63" s="28">
         <v>0.72726999999999997</v>
       </c>
-      <c r="I63" s="37"/>
+      <c r="I63" s="38"/>
     </row>
     <row r="64" spans="1:9" s="32" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A64" s="30" t="s">
@@ -2859,7 +2888,7 @@
       <c r="H64" s="31">
         <v>0.71291000000000004</v>
       </c>
-      <c r="I64" s="40"/>
+      <c r="I64" s="41"/>
     </row>
     <row r="65" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="21" t="s">
@@ -2886,7 +2915,7 @@
       <c r="H65" s="22">
         <v>0.76075999999999999</v>
       </c>
-      <c r="I65" s="41" t="s">
+      <c r="I65" s="42" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2915,7 +2944,7 @@
       <c r="H66" s="33">
         <v>0.77032999999999996</v>
       </c>
-      <c r="I66" s="35"/>
+      <c r="I66" s="36"/>
     </row>
     <row r="67" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="21" t="s">
@@ -2942,7 +2971,7 @@
       <c r="H67" s="33">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I67" s="35"/>
+      <c r="I67" s="36"/>
     </row>
     <row r="68" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="21" t="s">
@@ -2969,7 +2998,7 @@
       <c r="H68" s="33">
         <v>0.75597999999999999</v>
       </c>
-      <c r="I68" s="35"/>
+      <c r="I68" s="36"/>
     </row>
     <row r="69" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="21" t="s">
@@ -2996,7 +3025,7 @@
       <c r="H69" s="22">
         <v>0.73684000000000005</v>
       </c>
-      <c r="I69" s="35"/>
+      <c r="I69" s="36"/>
     </row>
     <row r="70" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="21" t="s">
@@ -3023,7 +3052,7 @@
       <c r="H70" s="24">
         <v>0.76554999999999995</v>
       </c>
-      <c r="I70" s="34" t="s">
+      <c r="I70" s="35" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3049,10 +3078,10 @@
       <c r="G71" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H71" s="24">
+      <c r="H71" s="49">
         <v>0.79425000000000001</v>
       </c>
-      <c r="I71" s="35"/>
+      <c r="I71" s="36"/>
     </row>
     <row r="72" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="21" t="s">
@@ -3079,7 +3108,7 @@
       <c r="H72" s="24">
         <v>0.77990000000000004</v>
       </c>
-      <c r="I72" s="35"/>
+      <c r="I72" s="36"/>
     </row>
     <row r="73" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="21" t="s">
@@ -3106,7 +3135,7 @@
       <c r="H73" s="24">
         <v>0.78468000000000004</v>
       </c>
-      <c r="I73" s="35"/>
+      <c r="I73" s="36"/>
     </row>
     <row r="74" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="21" t="s">
@@ -3133,7 +3162,7 @@
       <c r="H74" s="24">
         <v>0.77510999999999997</v>
       </c>
-      <c r="I74" s="35"/>
+      <c r="I74" s="36"/>
     </row>
     <row r="75" spans="1:9" s="23" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="21" t="s">
@@ -3160,10 +3189,254 @@
       <c r="H75" s="24">
         <v>0.78947000000000001</v>
       </c>
-      <c r="I75" s="35"/>
+      <c r="I75" s="36"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A76" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C76" s="14">
+        <v>300</v>
+      </c>
+      <c r="D76" s="14">
+        <v>10</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H76" s="14">
+        <v>0.77032999999999996</v>
+      </c>
+      <c r="I76" s="48"/>
+    </row>
+    <row r="77" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C77" s="14">
+        <v>50</v>
+      </c>
+      <c r="D77" s="14">
+        <v>10</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G77" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H77" s="14">
+        <v>0.75119000000000002</v>
+      </c>
+      <c r="I77" s="48"/>
+    </row>
+    <row r="78" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C78" s="14">
+        <v>100</v>
+      </c>
+      <c r="D78" s="14">
+        <v>10</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H78" s="14">
+        <v>0.75119000000000002</v>
+      </c>
+      <c r="I78" s="48"/>
+    </row>
+    <row r="79" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C79" s="14">
+        <v>200</v>
+      </c>
+      <c r="D79" s="14">
+        <v>10</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H79" s="47">
+        <v>0.77510999999999997</v>
+      </c>
+      <c r="I79" s="48"/>
+    </row>
+    <row r="80" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C80" s="14">
+        <v>230</v>
+      </c>
+      <c r="D80" s="14">
+        <v>10</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H80" s="47">
+        <v>0.77510999999999997</v>
+      </c>
+      <c r="I80" s="48"/>
+    </row>
+    <row r="81" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" s="14">
+        <v>240</v>
+      </c>
+      <c r="D81" s="14">
+        <v>10</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H81" s="47">
+        <v>0.77032999999999996</v>
+      </c>
+      <c r="I81" s="48"/>
+    </row>
+    <row r="82" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C82" s="14">
+        <v>260</v>
+      </c>
+      <c r="D82" s="14">
+        <v>10</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H82" s="47">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="I82" s="48"/>
+    </row>
+    <row r="83" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C83" s="14">
+        <v>280</v>
+      </c>
+      <c r="D83" s="14">
+        <v>10</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G83" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H83" s="14">
+        <v>0.75597999999999999</v>
+      </c>
+      <c r="I83" s="48"/>
+    </row>
+    <row r="84" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C84" s="14">
+        <v>290</v>
+      </c>
+      <c r="D84" s="14">
+        <v>10</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H84" s="14">
+        <v>0.77510999999999997</v>
+      </c>
+      <c r="I84" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="I76:I84"/>
     <mergeCell ref="I70:I75"/>
     <mergeCell ref="I35:I42"/>
     <mergeCell ref="I11:I22"/>
@@ -3194,15 +3467,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="42"/>
+      <c r="A1" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="43"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
@@ -3282,10 +3555,10 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="45"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">

</xml_diff>